<commit_message>
analises e resultados todos
</commit_message>
<xml_diff>
--- a/Exercício 3/Resultados/RNA FatigueLevel.xlsx
+++ b/Exercício 3/Resultados/RNA FatigueLevel.xlsx
@@ -349,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -466,22 +466,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -493,35 +484,29 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -530,6 +515,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -848,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AS75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AG4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -906,367 +897,367 @@
       <c r="C2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
       <c r="Q2" s="19"/>
     </row>
     <row r="3" spans="2:45" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="17"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
     </row>
     <row r="5" spans="2:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="G5" s="42" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="G5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="L5" s="42" t="s">
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="L5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="Q5" s="42" t="s">
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="Q5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="V5" s="42" t="s">
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="V5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="W5" s="42"/>
-      <c r="X5" s="42"/>
-      <c r="Y5" s="42"/>
-      <c r="AA5" s="42" t="s">
+      <c r="W5" s="51"/>
+      <c r="X5" s="51"/>
+      <c r="Y5" s="51"/>
+      <c r="AA5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="42"/>
-      <c r="AD5" s="42"/>
-      <c r="AF5" s="42" t="s">
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="51"/>
+      <c r="AF5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AG5" s="42"/>
-      <c r="AH5" s="42"/>
-      <c r="AI5" s="42"/>
-      <c r="AK5" s="42" t="s">
+      <c r="AG5" s="51"/>
+      <c r="AH5" s="51"/>
+      <c r="AI5" s="51"/>
+      <c r="AK5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AL5" s="42"/>
-      <c r="AM5" s="42"/>
-      <c r="AN5" s="42"/>
-      <c r="AP5" s="42" t="s">
+      <c r="AL5" s="51"/>
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="51"/>
+      <c r="AP5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AQ5" s="42"/>
-      <c r="AR5" s="42"/>
-      <c r="AS5" s="42"/>
+      <c r="AQ5" s="51"/>
+      <c r="AR5" s="51"/>
+      <c r="AS5" s="51"/>
     </row>
     <row r="6" spans="2:45" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="43"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="43"/>
-      <c r="J6" s="17" t="s">
+      <c r="I6" s="46"/>
+      <c r="J6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="17" t="s">
+      <c r="N6" s="46"/>
+      <c r="O6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="Q6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="43" t="s">
+      <c r="R6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="43"/>
-      <c r="T6" s="17" t="s">
+      <c r="S6" s="46"/>
+      <c r="T6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="V6" s="17" t="s">
+      <c r="V6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="W6" s="43" t="s">
+      <c r="W6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="X6" s="43"/>
-      <c r="Y6" s="17" t="s">
+      <c r="X6" s="46"/>
+      <c r="Y6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AA6" s="17" t="s">
+      <c r="AA6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="AB6" s="43" t="s">
+      <c r="AB6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="AC6" s="43"/>
-      <c r="AD6" s="17" t="s">
+      <c r="AC6" s="46"/>
+      <c r="AD6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AF6" s="17" t="s">
+      <c r="AF6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="AG6" s="43" t="s">
+      <c r="AG6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="AH6" s="43"/>
-      <c r="AI6" s="17" t="s">
+      <c r="AH6" s="46"/>
+      <c r="AI6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AK6" s="17" t="s">
+      <c r="AK6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="AL6" s="43" t="s">
+      <c r="AL6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="AM6" s="43"/>
-      <c r="AN6" s="17" t="s">
+      <c r="AM6" s="46"/>
+      <c r="AN6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AP6" s="17" t="s">
+      <c r="AP6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="AQ6" s="43" t="s">
+      <c r="AQ6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="AR6" s="43"/>
-      <c r="AS6" s="17" t="s">
+      <c r="AR6" s="46"/>
+      <c r="AS6" s="41" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:45" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="18" t="e">
-        <f>INDEX(B10:E10,MATCH(C7,C10:C74,0),1)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C7" s="44">
+      <c r="B7" s="18" t="str">
+        <f>INDEX(B10:E74,MATCH(C7,C10:C74,0),1)</f>
+        <v>5,4,3</v>
+      </c>
+      <c r="C7" s="42">
         <f>MIN(C10:C74)</f>
         <v>1.1121296380000001</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="18" t="e">
-        <f>INDEX(B10:E10,MATCH(C7,C10:C74,0),4)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G7" s="18">
-        <f>INDEX(G10:J10,MATCH(H7,H10:H74,0),1)</f>
+      <c r="D7" s="42"/>
+      <c r="E7" s="18">
+        <f>INDEX(B10:E74,MATCH(C7,C10:C74,0),4)</f>
+        <v>313.50240000000002</v>
+      </c>
+      <c r="G7" s="40">
+        <f>INDEX(G10:J74,MATCH(H7,H10:H74,0),1)</f>
         <v>2.1</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="42">
         <f>MIN(H10:H74)</f>
         <v>1.1003266650000001</v>
       </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="18">
-        <f>INDEX(G10:J10,MATCH(H7,H10:H74,0),4)</f>
+      <c r="I7" s="42"/>
+      <c r="J7" s="40">
+        <f>INDEX(G10:J74,MATCH(H7,H10:H74,0),4)</f>
         <v>292.53267</v>
       </c>
-      <c r="L7" s="18" t="e">
-        <f>INDEX(L10:O10,MATCH(M7,M10:M74,0),1)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M7" s="44">
+      <c r="L7" s="40" t="str">
+        <f>INDEX(L10:O74,MATCH(M7,M10:M74,0),1)</f>
+        <v>5,4,2</v>
+      </c>
+      <c r="M7" s="42">
         <f>MIN(M10:M74)</f>
         <v>1.1274823730000001</v>
       </c>
-      <c r="N7" s="44"/>
-      <c r="O7" s="18" t="e">
-        <f>INDEX(L10:O10,MATCH(M7,M10:M74,0),4)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q7" s="18" t="str">
-        <f>INDEX(Q10:T10,MATCH(R7,R10:R74,0),1)</f>
+      <c r="N7" s="42"/>
+      <c r="O7" s="40">
+        <f>INDEX(L10:O74,MATCH(M7,M10:M74,0),4)</f>
+        <v>248.15683000000001</v>
+      </c>
+      <c r="Q7" s="40" t="str">
+        <f>INDEX(Q10:T74,MATCH(R7,R10:R74,0),1)</f>
         <v>5,3,2</v>
       </c>
-      <c r="R7" s="45">
+      <c r="R7" s="42">
         <f>MIN(R10:R74)</f>
         <v>1.1173482779999999</v>
       </c>
-      <c r="S7" s="45"/>
-      <c r="T7" s="18">
-        <f>INDEX(Q10:T10,MATCH(R7,R10:R74,0),4)</f>
+      <c r="S7" s="42"/>
+      <c r="T7" s="40">
+        <f>INDEX(Q10:T74,MATCH(R7,R10:R74,0),4)</f>
         <v>245.24816000000001</v>
       </c>
       <c r="U7" s="5"/>
-      <c r="V7" s="18">
-        <f>INDEX(V10:Y10,MATCH(W7,W10:W74,0),1)</f>
+      <c r="V7" s="40">
+        <f>INDEX(V10:Y74,MATCH(W7,W10:W74,0),1)</f>
         <v>4.3</v>
       </c>
-      <c r="W7" s="45">
+      <c r="W7" s="42">
         <f>MIN(W10:W74)</f>
         <v>1.1239005070000001</v>
       </c>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="18">
-        <f>INDEX(V10:Y10,MATCH(W7,W10:W74,0),4)</f>
+      <c r="X7" s="42"/>
+      <c r="Y7" s="40">
+        <f>INDEX(V10:Y74,MATCH(W7,W10:W74,0),4)</f>
         <v>221.04112000000001</v>
       </c>
-      <c r="AA7" s="18">
-        <f>INDEX(AA10:AD10,MATCH(AB7,AB10:AB74,0),1)</f>
+      <c r="AA7" s="40">
+        <f>INDEX(AA10:AD74,MATCH(AB7,AB10:AB74,0),1)</f>
         <v>4.3</v>
       </c>
-      <c r="AB7" s="45">
+      <c r="AB7" s="42">
         <f>MIN(AB10:AB74)</f>
         <v>1.1232752180000001</v>
       </c>
-      <c r="AC7" s="45"/>
-      <c r="AD7" s="18">
-        <f>INDEX(AA10:AD10,MATCH(AB7,AB10:AB74,0),4)</f>
+      <c r="AC7" s="42"/>
+      <c r="AD7" s="40">
+        <f>INDEX(AA10:AD74,MATCH(AB7,AB10:AB74,0),4)</f>
         <v>220.48066</v>
       </c>
-      <c r="AF7" s="18">
-        <f>INDEX(AF10:AI10,MATCH(AG7,AG10:AG74,0),1)</f>
+      <c r="AF7" s="40">
+        <f>INDEX(AF10:AI74,MATCH(AG7,AG10:AG74,0),1)</f>
         <v>6.6</v>
       </c>
-      <c r="AG7" s="44">
+      <c r="AG7" s="42">
         <f>MIN(AG10:AG74)</f>
         <v>1.299102499</v>
       </c>
-      <c r="AH7" s="44"/>
-      <c r="AI7" s="10">
-        <f>INDEX(AF10:AI10,MATCH(AG7,AG10:AG74,0),4)</f>
+      <c r="AH7" s="42"/>
+      <c r="AI7" s="40">
+        <f>INDEX(AF10:AI74,MATCH(AG7,AG10:AG74,0),4)</f>
         <v>150.76866000000001</v>
       </c>
-      <c r="AK7" s="18" t="e">
-        <f>INDEX(AK10:AN10,MATCH(AL7,AL10:AL74,0),1)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AL7" s="44">
+      <c r="AK7" s="40">
+        <f>INDEX(AK10:AN74,MATCH(AL7,AL10:AL74,0),1)</f>
+        <v>3.2</v>
+      </c>
+      <c r="AL7" s="42">
         <f>MIN(AL10:AL74)</f>
         <v>1.182429204</v>
       </c>
-      <c r="AM7" s="44"/>
-      <c r="AN7" s="10" t="e">
-        <f>INDEX(AK10:AN10,MATCH(AL7,AL10:AL74,0),4)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AP7" s="18" t="e">
-        <f>INDEX(AP10:AS10,MATCH(AQ7,AQ10:AQ74,0),1)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AQ7" s="44">
+      <c r="AM7" s="42"/>
+      <c r="AN7" s="40">
+        <f>INDEX(AK10:AN74,MATCH(AL7,AL10:AL74,0),4)</f>
+        <v>251.44973999999999</v>
+      </c>
+      <c r="AP7" s="40" t="str">
+        <f>INDEX(AP10:AS74,MATCH(AQ7,AQ10:AQ74,0),1)</f>
+        <v>3,2,1</v>
+      </c>
+      <c r="AQ7" s="42">
         <f>MIN(AQ10:AQ74)</f>
         <v>1.1223383870000001</v>
       </c>
-      <c r="AR7" s="44"/>
-      <c r="AS7" s="10" t="e">
-        <f>INDEX(AP10:AS10,MATCH(AQ7,AQ10:AQ74,0),4)</f>
-        <v>#REF!</v>
+      <c r="AR7" s="42"/>
+      <c r="AS7" s="40">
+        <f>INDEX(AP10:AS74,MATCH(AQ7,AQ10:AQ74,0),4)</f>
+        <v>240.91255000000001</v>
       </c>
     </row>
     <row r="8" spans="2:45" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="19"/>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="45"/>
       <c r="K8" s="24"/>
-      <c r="L8" s="46" t="s">
+      <c r="L8" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="48"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="45"/>
       <c r="P8" s="24"/>
-      <c r="Q8" s="46" t="s">
+      <c r="Q8" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="48"/>
-      <c r="V8" s="46" t="s">
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="45"/>
+      <c r="V8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="W8" s="47"/>
-      <c r="X8" s="47"/>
-      <c r="Y8" s="48"/>
-      <c r="AA8" s="46" t="s">
+      <c r="W8" s="44"/>
+      <c r="X8" s="44"/>
+      <c r="Y8" s="45"/>
+      <c r="AA8" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="AB8" s="47"/>
-      <c r="AC8" s="47"/>
-      <c r="AD8" s="48"/>
-      <c r="AF8" s="49" t="s">
+      <c r="AB8" s="44"/>
+      <c r="AC8" s="44"/>
+      <c r="AD8" s="45"/>
+      <c r="AF8" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="AG8" s="50"/>
-      <c r="AH8" s="50"/>
-      <c r="AI8" s="51"/>
-      <c r="AK8" s="49" t="s">
+      <c r="AG8" s="48"/>
+      <c r="AH8" s="48"/>
+      <c r="AI8" s="50"/>
+      <c r="AK8" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="AL8" s="50"/>
-      <c r="AM8" s="52"/>
-      <c r="AN8" s="51"/>
-      <c r="AP8" s="49" t="s">
+      <c r="AL8" s="48"/>
+      <c r="AM8" s="49"/>
+      <c r="AN8" s="50"/>
+      <c r="AP8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="AQ8" s="52"/>
-      <c r="AR8" s="52"/>
-      <c r="AS8" s="51"/>
+      <c r="AQ8" s="49"/>
+      <c r="AR8" s="49"/>
+      <c r="AS8" s="50"/>
     </row>
     <row r="9" spans="2:45" x14ac:dyDescent="0.15">
       <c r="B9" s="13" t="s">
@@ -4052,44 +4043,44 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="AP8:AS8"/>
-    <mergeCell ref="AG7:AH7"/>
-    <mergeCell ref="AL7:AM7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="Q8:T8"/>
-    <mergeCell ref="V8:Y8"/>
-    <mergeCell ref="AA8:AD8"/>
-    <mergeCell ref="AF8:AI8"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AL6:AM6"/>
-    <mergeCell ref="AK8:AN8"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="AF5:AI5"/>
-    <mergeCell ref="AK5:AN5"/>
-    <mergeCell ref="AP5:AS5"/>
     <mergeCell ref="D2:P2"/>
     <mergeCell ref="C3:Q3"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="AF5:AI5"/>
+    <mergeCell ref="AK5:AN5"/>
+    <mergeCell ref="AP5:AS5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AL6:AM6"/>
+    <mergeCell ref="AK8:AN8"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AP8:AS8"/>
+    <mergeCell ref="AG7:AH7"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AA8:AD8"/>
+    <mergeCell ref="AF8:AI8"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="W7:X7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4099,8 +4090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AN74"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView showGridLines="0" topLeftCell="U1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5:Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -4157,332 +4148,332 @@
       <c r="C2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
       <c r="Q2" s="31"/>
     </row>
     <row r="3" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="33"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
     </row>
     <row r="5" spans="2:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="G5" s="55" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="G5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="L5" s="55" t="s">
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="L5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="Q5" s="55" t="s">
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="Q5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="55"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="V5" s="55" t="s">
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="V5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="W5" s="55"/>
-      <c r="X5" s="55"/>
-      <c r="Y5" s="55"/>
-      <c r="AA5" s="55" t="s">
+      <c r="W5" s="51"/>
+      <c r="X5" s="51"/>
+      <c r="Y5" s="51"/>
+      <c r="AA5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AB5" s="55"/>
-      <c r="AC5" s="55"/>
-      <c r="AD5" s="55"/>
-      <c r="AF5" s="55" t="s">
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="51"/>
+      <c r="AF5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AG5" s="55"/>
-      <c r="AH5" s="55"/>
-      <c r="AI5" s="55"/>
-      <c r="AK5" s="55" t="s">
+      <c r="AG5" s="51"/>
+      <c r="AH5" s="51"/>
+      <c r="AI5" s="51"/>
+      <c r="AK5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AL5" s="55"/>
-      <c r="AM5" s="55"/>
-      <c r="AN5" s="55"/>
+      <c r="AL5" s="51"/>
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="51"/>
     </row>
     <row r="6" spans="2:40" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="33" t="s">
+      <c r="D6" s="46"/>
+      <c r="E6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="33" t="s">
+      <c r="I6" s="46"/>
+      <c r="J6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="56" t="s">
+      <c r="M6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="56"/>
-      <c r="O6" s="33" t="s">
+      <c r="N6" s="46"/>
+      <c r="O6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="33" t="s">
+      <c r="Q6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="56" t="s">
+      <c r="R6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="56"/>
-      <c r="T6" s="33" t="s">
+      <c r="S6" s="46"/>
+      <c r="T6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="V6" s="33" t="s">
+      <c r="V6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="W6" s="56" t="s">
+      <c r="W6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="X6" s="56"/>
-      <c r="Y6" s="33" t="s">
+      <c r="X6" s="46"/>
+      <c r="Y6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AA6" s="33" t="s">
+      <c r="AA6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="AB6" s="56" t="s">
+      <c r="AB6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="AC6" s="56"/>
-      <c r="AD6" s="33" t="s">
+      <c r="AC6" s="46"/>
+      <c r="AD6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AF6" s="33" t="s">
+      <c r="AF6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="AG6" s="56" t="s">
+      <c r="AG6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="AH6" s="56"/>
-      <c r="AI6" s="33" t="s">
+      <c r="AH6" s="46"/>
+      <c r="AI6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AK6" s="33" t="s">
+      <c r="AK6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="AL6" s="56" t="s">
+      <c r="AL6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="AM6" s="56"/>
-      <c r="AN6" s="33" t="s">
+      <c r="AM6" s="46"/>
+      <c r="AN6" s="41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:40" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="29">
-        <f>INDEX(B10:E10,MATCH(C7,C10:C74,0),1)</f>
+    <row r="7" spans="2:40" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="40">
+        <f>INDEX(B10:E74,MATCH(C7,C10:C74,0),1)</f>
         <v>5.4</v>
       </c>
-      <c r="C7" s="57">
+      <c r="C7" s="42">
         <f>MIN(C10:C74)</f>
         <v>0.3889813707</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="29">
-        <f>INDEX(B10:E10,MATCH(C7,C10:C74,0),4)</f>
+      <c r="D7" s="42"/>
+      <c r="E7" s="40">
+        <f>INDEX(B10:E74,MATCH(C7,C10:C74,0),4)</f>
         <v>40.097250000000003</v>
       </c>
-      <c r="G7" s="29" t="e">
-        <f>INDEX(G10:J10,MATCH(H7,H10:H74,0),1)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H7" s="57">
+      <c r="G7" s="40" t="str">
+        <f>INDEX(G10:J74,MATCH(H7,H10:H74,0),1)</f>
+        <v>4,3,2</v>
+      </c>
+      <c r="H7" s="42">
         <f>MIN(H10:H74)</f>
         <v>0.38959069829999998</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="29" t="e">
-        <f>INDEX(G10:J10,MATCH(H7,H10:H74,0),4)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L7" s="29">
-        <f>INDEX(L10:O10,MATCH(M7,M10:M74,0),1)</f>
+      <c r="I7" s="42"/>
+      <c r="J7" s="40">
+        <f>INDEX(G10:J74,MATCH(H7,H10:H74,0),4)</f>
+        <v>39.85239</v>
+      </c>
+      <c r="L7" s="40">
+        <f>INDEX(L10:O74,MATCH(M7,M10:M74,0),1)</f>
         <v>4.3</v>
       </c>
-      <c r="M7" s="57">
+      <c r="M7" s="42">
         <f>MIN(M10:M74)</f>
         <v>0.4125550281</v>
       </c>
-      <c r="N7" s="57"/>
-      <c r="O7" s="29">
-        <f>INDEX(L10:O10,MATCH(M7,M10:M74,0),4)</f>
+      <c r="N7" s="42"/>
+      <c r="O7" s="40">
+        <f>INDEX(L10:O74,MATCH(M7,M10:M74,0),4)</f>
         <v>34.371720000000003</v>
       </c>
-      <c r="Q7" s="29">
-        <f>INDEX(Q10:T10,MATCH(R7,R10:R74,0),1)</f>
+      <c r="Q7" s="40">
+        <f>INDEX(Q10:T74,MATCH(R7,R10:R74,0),1)</f>
         <v>7.2</v>
       </c>
-      <c r="R7" s="58">
+      <c r="R7" s="42">
         <f>MIN(R10:R74)</f>
         <v>0.41667431100000002</v>
       </c>
-      <c r="S7" s="58"/>
-      <c r="T7" s="29">
-        <f>INDEX(Q10:T10,MATCH(R7,R10:R74,0),4)</f>
+      <c r="S7" s="42"/>
+      <c r="T7" s="40">
+        <f>INDEX(Q10:T74,MATCH(R7,R10:R74,0),4)</f>
         <v>31.184380000000001</v>
       </c>
       <c r="U7" s="3"/>
-      <c r="V7" s="29">
-        <f>INDEX(V10:Y10,MATCH(W7,W10:W74,0),1)</f>
+      <c r="V7" s="40">
+        <f>INDEX(V10:Y74,MATCH(W7,W10:W74,0),1)</f>
         <v>4.3</v>
       </c>
-      <c r="W7" s="58">
+      <c r="W7" s="42">
         <f>MIN(W10:W74)</f>
         <v>0.4164734424</v>
       </c>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="29">
-        <f>INDEX(V10:Y10,MATCH(W7,W10:W74,0),4)</f>
+      <c r="X7" s="42"/>
+      <c r="Y7" s="40">
+        <f>INDEX(V10:Y74,MATCH(W7,W10:W74,0),4)</f>
         <v>32.281109999999998</v>
       </c>
-      <c r="AA7" s="29" t="e">
-        <f>INDEX(AA10:AD10,MATCH(AB7,AB10:AB74,0),1)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AB7" s="58">
+      <c r="AA7" s="40">
+        <f>INDEX(AA10:AD74,MATCH(AB7,AB10:AB74,0),1)</f>
+        <v>5.4</v>
+      </c>
+      <c r="AB7" s="42">
         <f>MIN(AB10:AB74)</f>
         <v>0.44420379850000002</v>
       </c>
-      <c r="AC7" s="58"/>
-      <c r="AD7" s="29" t="e">
-        <f>INDEX(AA10:AD10,MATCH(AB7,AB10:AB74,0),4)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AF7" s="29">
-        <f>INDEX(AF10:AI10,MATCH(AG7,AG10:AG74,0),1)</f>
+      <c r="AC7" s="42"/>
+      <c r="AD7" s="40">
+        <f>INDEX(AA10:AD74,MATCH(AB7,AB10:AB74,0),4)</f>
+        <v>27.955480000000001</v>
+      </c>
+      <c r="AF7" s="40">
+        <f>INDEX(AF10:AI74,MATCH(AG7,AG10:AG74,0),1)</f>
         <v>5.4</v>
       </c>
-      <c r="AG7" s="57">
+      <c r="AG7" s="42">
         <f>MIN(AG10:AG74)</f>
         <v>0.45989743459999999</v>
       </c>
-      <c r="AH7" s="57"/>
-      <c r="AI7" s="34">
-        <f>INDEX(AF10:AI10,MATCH(AG7,AG10:AG74,0),4)</f>
+      <c r="AH7" s="42"/>
+      <c r="AI7" s="40">
+        <f>INDEX(AF10:AI74,MATCH(AG7,AG10:AG74,0),4)</f>
         <v>26.50093</v>
       </c>
-      <c r="AK7" s="29" t="e">
-        <f>INDEX(AK10:AN10,MATCH(AL7,AL10:AL74,0),1)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AL7" s="57">
+      <c r="AK7" s="40">
+        <f>INDEX(AK10:AN74,MATCH(AL7,AL10:AL74,0),1)</f>
+        <v>7.5</v>
+      </c>
+      <c r="AL7" s="42">
         <f>MIN(AL10:AL74)</f>
         <v>0.46122735910000001</v>
       </c>
-      <c r="AM7" s="57"/>
-      <c r="AN7" s="34" t="e">
-        <f>INDEX(AK10:AN10,MATCH(AL7,AL10:AL74,0),4)</f>
-        <v>#REF!</v>
+      <c r="AM7" s="42"/>
+      <c r="AN7" s="40">
+        <f>INDEX(AK10:AN74,MATCH(AL7,AL10:AL74,0),4)</f>
+        <v>16.671029999999998</v>
       </c>
     </row>
     <row r="8" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="61"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="31"/>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
       <c r="K8" s="35"/>
-      <c r="L8" s="59" t="s">
+      <c r="L8" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="61"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="56"/>
       <c r="P8" s="35"/>
-      <c r="Q8" s="59" t="s">
+      <c r="Q8" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="61"/>
-      <c r="V8" s="59" t="s">
+      <c r="R8" s="55"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="56"/>
+      <c r="V8" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="W8" s="60"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="61"/>
-      <c r="AA8" s="59" t="s">
+      <c r="W8" s="55"/>
+      <c r="X8" s="55"/>
+      <c r="Y8" s="56"/>
+      <c r="AA8" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AB8" s="60"/>
-      <c r="AC8" s="60"/>
-      <c r="AD8" s="61"/>
-      <c r="AF8" s="59" t="s">
+      <c r="AB8" s="55"/>
+      <c r="AC8" s="55"/>
+      <c r="AD8" s="56"/>
+      <c r="AF8" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="AG8" s="60"/>
-      <c r="AH8" s="60"/>
-      <c r="AI8" s="61"/>
-      <c r="AK8" s="59" t="s">
+      <c r="AG8" s="55"/>
+      <c r="AH8" s="55"/>
+      <c r="AI8" s="56"/>
+      <c r="AK8" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="AL8" s="60"/>
-      <c r="AM8" s="60"/>
-      <c r="AN8" s="61"/>
+      <c r="AL8" s="55"/>
+      <c r="AM8" s="55"/>
+      <c r="AN8" s="56"/>
     </row>
     <row r="9" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
@@ -7151,6 +7142,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="D2:P2"/>
+    <mergeCell ref="C3:Q3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="AF5:AI5"/>
+    <mergeCell ref="AK5:AN5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AL6:AM6"/>
     <mergeCell ref="AB7:AC7"/>
     <mergeCell ref="AK8:AN8"/>
     <mergeCell ref="AG7:AH7"/>
@@ -7167,24 +7176,6 @@
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="W7:X7"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="AF5:AI5"/>
-    <mergeCell ref="AK5:AN5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AL6:AM6"/>
-    <mergeCell ref="D2:P2"/>
-    <mergeCell ref="C3:Q3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="Q5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>